<commit_message>
Update Skills England Occupational Standards Data Attribution Statements
</commit_message>
<xml_diff>
--- a/SSC - Mappings - Digital Skills - v0.9.1 - 20251124.xlsx
+++ b/SSC - Mappings - Digital Skills - v0.9.1 - 20251124.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilb\Documents\Omifolio\Research\IER\Skills Project\SSC Phase 2\v0.9.1\SSCE Download Versions - 20251112\Final\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neilb\Documents\GitHub\ddfiles202511\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F76096F-6FF0-417D-A1FE-87C609EF8F5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBAC8369-44DC-44CA-8224-6FCA08B0ADA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{428CD01E-E34D-408E-A3C5-98FC21288E3C}"/>
   </bookViews>
@@ -30207,10 +30207,10 @@
     <t xml:space="preserve">2) Version 1.2 of the ESCO classification of the European Commission, used under the CC BY 4.0 license (Source https://esco.ec.europa.eu/) </t>
   </si>
   <si>
-    <t>3) Skills England Occupational Standards (provided by IfATE), used under the CC BY 4.0 license (Source: https://www.gov.uk/government/organisations/skills-england)</t>
-  </si>
-  <si>
     <t>5) AGCAS graduate career profiles, used under a custom license. (Source: https://www.prospects.ac.uk/); copyright holders are AGCAS (The Association of Graduate Careers Advisory Services)</t>
+  </si>
+  <si>
+    <t>3) Skills England Occupational Standards (provided by IfATE from the Standards API), used under the Open Government Licence v3.0 (Source: https://www.gov.uk/government/organisations/skills-england)</t>
   </si>
 </sst>
 </file>
@@ -30865,7 +30865,7 @@
     </row>
     <row r="14" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
-        <v>10053</v>
+        <v>10054</v>
       </c>
     </row>
     <row r="15" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
@@ -30875,7 +30875,7 @@
     </row>
     <row r="16" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12" t="s">
-        <v>10054</v>
+        <v>10053</v>
       </c>
     </row>
     <row r="17" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2"/>

</xml_diff>